<commit_message>
add project_plan_week_1 update assigned to
</commit_message>
<xml_diff>
--- a/Documents/Weekly Plan/Project Plan.xlsx
+++ b/Documents/Weekly Plan/Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudangkhoa/Documents/EduPKA/Documents/Weekly Plan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2187858-9737-F24F-AF96-EAC83BD531C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DD8F3D-F2E7-7F4A-AB99-796AF40ADD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="71">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t>Lên kế hoạch cơ sở dữ liệu</t>
+  </si>
+  <si>
+    <t>Vũ Đăng Khoa / Trịnh Văn Toàn</t>
+  </si>
+  <si>
+    <t>Toàn bộ thành viên</t>
   </si>
 </sst>
 </file>
@@ -655,7 +661,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -933,6 +939,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.59996337778862885"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -964,7 +992,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1346,6 +1374,15 @@
     </xf>
     <xf numFmtId="164" fontId="19" fillId="5" borderId="24" xfId="10" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="25" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="26" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -3023,15 +3060,15 @@
   </sheetPr>
   <dimension ref="A1:BL32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="109" zoomScaleNormal="64" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="109" zoomScaleNormal="64" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="13" customWidth="1"/>
     <col min="2" max="2" width="51.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
@@ -3905,7 +3942,9 @@
       <c r="B12" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="48"/>
+      <c r="C12" s="138" t="s">
+        <v>61</v>
+      </c>
       <c r="D12" s="49">
         <v>1</v>
       </c>
@@ -3984,7 +4023,9 @@
       <c r="B13" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="53"/>
+      <c r="C13" s="140" t="s">
+        <v>70</v>
+      </c>
       <c r="D13" s="54">
         <v>0.6</v>
       </c>
@@ -4063,7 +4104,9 @@
       <c r="B14" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="53"/>
+      <c r="C14" s="139" t="s">
+        <v>69</v>
+      </c>
       <c r="D14" s="54">
         <v>1</v>
       </c>
@@ -4142,7 +4185,9 @@
       <c r="B15" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="53"/>
+      <c r="C15" s="53" t="s">
+        <v>61</v>
+      </c>
       <c r="D15" s="54">
         <v>0.75</v>
       </c>
@@ -4302,7 +4347,9 @@
       <c r="B18" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="63"/>
+      <c r="C18" s="63" t="s">
+        <v>61</v>
+      </c>
       <c r="D18" s="64">
         <v>0.5</v>
       </c>
@@ -4380,7 +4427,9 @@
       <c r="B19" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="63"/>
+      <c r="C19" s="63" t="s">
+        <v>70</v>
+      </c>
       <c r="D19" s="133">
         <v>0.9</v>
       </c>
@@ -4455,7 +4504,9 @@
       <c r="B20" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="63"/>
+      <c r="C20" s="63" t="s">
+        <v>70</v>
+      </c>
       <c r="D20" s="64">
         <v>0.95</v>
       </c>
@@ -4534,7 +4585,9 @@
       <c r="B21" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="63"/>
+      <c r="C21" s="63" t="s">
+        <v>70</v>
+      </c>
       <c r="D21" s="64">
         <v>1</v>
       </c>
@@ -4628,7 +4681,9 @@
       <c r="B23" s="114" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="115"/>
+      <c r="C23" s="115" t="s">
+        <v>61</v>
+      </c>
       <c r="D23" s="116">
         <v>0.45</v>
       </c>
@@ -4707,7 +4762,9 @@
       <c r="B24" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="115"/>
+      <c r="C24" s="115" t="s">
+        <v>61</v>
+      </c>
       <c r="D24" s="116">
         <v>0.25</v>
       </c>
@@ -4783,7 +4840,9 @@
       <c r="B25" s="114" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="115"/>
+      <c r="C25" s="115" t="s">
+        <v>61</v>
+      </c>
       <c r="D25" s="116">
         <v>1</v>
       </c>
@@ -4933,7 +4992,9 @@
       <c r="B27" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="73"/>
+      <c r="C27" s="73" t="s">
+        <v>70</v>
+      </c>
       <c r="D27" s="74">
         <v>0.15</v>
       </c>
@@ -5012,7 +5073,9 @@
       <c r="B28" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="73"/>
+      <c r="C28" s="73" t="s">
+        <v>70</v>
+      </c>
       <c r="D28" s="74">
         <v>0.3</v>
       </c>
@@ -5090,7 +5153,9 @@
       <c r="B29" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="73"/>
+      <c r="C29" s="73" t="s">
+        <v>61</v>
+      </c>
       <c r="D29" s="74">
         <v>1</v>
       </c>

</xml_diff>